<commit_message>
updated  testdata.xls in PageObject model
</commit_message>
<xml_diff>
--- a/PageObjectModel/src/test/resources/excel/testdata.xlsx
+++ b/PageObjectModel/src/test/resources/excel/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AutomationFramework\PageObjectModel\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B892786A-5EB6-47D8-9568-768C471C4493}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5B7F484-A86D-4FE7-9594-242AB3FF3E23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{4EE8F7EA-477F-4DEF-A3DC-0173AE102C5D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4EE8F7EA-477F-4DEF-A3DC-0173AE102C5D}"/>
   </bookViews>
   <sheets>
     <sheet name="findNewCarTest" sheetId="5" r:id="rId1"/>
@@ -67,10 +67,10 @@
     <t>Toyota Cars</t>
   </si>
   <si>
-    <t>Ho Cars</t>
-  </si>
-  <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>Honda Cars</t>
   </si>
 </sst>
 </file>
@@ -424,8 +424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB4E1D71-2A7B-4AA4-9C07-289CF2BC5396}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -473,7 +473,7 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -513,7 +513,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87BC0743-AC36-4433-9336-83061BACE965}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3:B5"/>
     </sheetView>
   </sheetViews>
@@ -535,7 +535,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -546,7 +546,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -557,7 +557,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
@@ -568,7 +568,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Test cases run mode updated in Page Object Model
</commit_message>
<xml_diff>
--- a/PageObjectModel/src/test/resources/excel/testdata.xlsx
+++ b/PageObjectModel/src/test/resources/excel/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AutomationFramework\PageObjectModel\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5B7F484-A86D-4FE7-9594-242AB3FF3E23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49F8F50A-0C80-421D-BE71-65D8E4E2255C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4EE8F7EA-477F-4DEF-A3DC-0173AE102C5D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{4EE8F7EA-477F-4DEF-A3DC-0173AE102C5D}"/>
   </bookViews>
   <sheets>
     <sheet name="findNewCarTest" sheetId="5" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="14">
   <si>
     <t>browser</t>
   </si>
@@ -65,9 +65,6 @@
   </si>
   <si>
     <t>Toyota Cars</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
   <si>
     <t>Honda Cars</t>
@@ -424,8 +421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB4E1D71-2A7B-4AA4-9C07-289CF2BC5396}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -473,7 +470,7 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -513,8 +510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87BC0743-AC36-4433-9336-83061BACE965}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -535,7 +532,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -546,7 +543,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -557,7 +554,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
@@ -568,7 +565,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Mail sending functionality added
</commit_message>
<xml_diff>
--- a/PageObjectModel/src/test/resources/excel/testdata.xlsx
+++ b/PageObjectModel/src/test/resources/excel/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AutomationFramework\PageObjectModel\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49F8F50A-0C80-421D-BE71-65D8E4E2255C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EBEB3AE-CAE2-40F7-BEF6-B15C74D0EC3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{4EE8F7EA-477F-4DEF-A3DC-0173AE102C5D}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="16">
   <si>
     <t>browser</t>
   </si>
@@ -68,6 +68,12 @@
   </si>
   <si>
     <t>Honda Cars</t>
+  </si>
+  <si>
+    <t>tata</t>
+  </si>
+  <si>
+    <t>Tata Cars</t>
   </si>
 </sst>
 </file>
@@ -419,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB4E1D71-2A7B-4AA4-9C07-289CF2BC5396}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="S9" sqref="S1:X9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -467,10 +473,10 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -481,10 +487,10 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -495,10 +501,24 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -508,10 +528,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87BC0743-AC36-4433-9336-83061BACE965}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -571,6 +591,17 @@
         <v>7</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>